<commit_message>
Confirm names to use for geodatabase aliases
Per 2025-02-06 team meeting
</commit_message>
<xml_diff>
--- a/data/Survey123_Field Names and Aliases_20241220.xlsx
+++ b/data/Survey123_Field Names and Aliases_20241220.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isbcf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\manniongeo\projects\nwfwmd\2015-01-13_gis_support\github\Hydrologic-Monitoring-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACA1C3A-69BD-481C-B44F-00D7016A3A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767117A1-E176-4288-B196-3E784332CF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2EC705E7-C833-41D9-B7F8-0755F5ED5DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21330" xr2:uid="{2EC705E7-C833-41D9-B7F8-0755F5ED5DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>tc={27CC4477-F44C-47C1-9E73-E0CC9835FE6C}</author>
   </authors>
   <commentList>
-    <comment ref="F87" authorId="0" shapeId="0" xr:uid="{27CC4477-F44C-47C1-9E73-E0CC9835FE6C}">
+    <comment ref="F119" authorId="0" shapeId="0" xr:uid="{27CC4477-F44C-47C1-9E73-E0CC9835FE6C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="243">
   <si>
     <t>VisitDate</t>
   </si>
@@ -676,9 +676,6 @@
     <t>PARAMETER</t>
   </si>
   <si>
-    <t>Battery Replacement Exceptio</t>
-  </si>
-  <si>
     <t>Data Logger Time Difference (minutes)</t>
   </si>
   <si>
@@ -700,9 +697,6 @@
     <t>Survey123 Data Type</t>
   </si>
   <si>
-    <t>Specific Conductance sensor failed</t>
-  </si>
-  <si>
     <t>Conductivity Sensor Adjustment Comments</t>
   </si>
   <si>
@@ -782,6 +776,15 @@
   </si>
   <si>
     <t>Calibration Date</t>
+  </si>
+  <si>
+    <t>Use "Aquarius Label in Comments"</t>
+  </si>
+  <si>
+    <t>Specific Conductance Sensor Failed</t>
+  </si>
+  <si>
+    <t>Keep existing geodatabase aliases</t>
   </si>
 </sst>
 </file>
@@ -852,7 +855,182 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -869,6 +1047,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -890,13 +1074,13 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A90A420-8FA1-4456-9A8A-729261121E4A}" name="Table1" displayName="Table1" ref="A1:G152" totalsRowShown="0">
   <autoFilter ref="A1:G152" xr:uid="{1A90A420-8FA1-4456-9A8A-729261121E4A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G152">
-    <sortCondition ref="D1:D152"/>
+    <sortCondition ref="A1:A152"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{AD386C89-A8CF-47ED-A525-B12B7ED4BE80}" name="Survey123 Table (sql-gis &gt; hydro)"/>
     <tableColumn id="2" xr3:uid="{AABE8E1B-B8EB-4685-8A16-78EB19DF3895}" name="Survey123 Field Name"/>
     <tableColumn id="3" xr3:uid="{596E73BB-6FFC-4A91-AAB7-F6CB517170C0}" name="Survey123 Alias"/>
-    <tableColumn id="7" xr3:uid="{089A2009-3B44-4F53-B9F6-4F500D1CB88B}" name="Changes to Survey123 Alias" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{089A2009-3B44-4F53-B9F6-4F500D1CB88B}" name="Changes to Survey123 Alias" dataDxfId="17"/>
     <tableColumn id="4" xr3:uid="{241C2369-5EDD-4416-A799-35B3CC6568FC}" name="Survey123 Data Type"/>
     <tableColumn id="5" xr3:uid="{61DEC2AB-0028-4608-B234-E86C8A78F6E5}" name="Aquarius Label in Comments"/>
     <tableColumn id="6" xr3:uid="{CCA2A3E5-5D9F-4987-BFBD-DE5D29943122}" name="Note"/>
@@ -1222,10 +1406,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F87" dT="2024-12-19T20:36:59.99" personId="{B66E1D1B-CB7D-4B58-9430-5B21786DE2E6}" id="{27CC4477-F44C-47C1-9E73-E0CC9835FE6C}">
+  <threadedComment ref="F119" dT="2024-12-19T20:36:59.99" personId="{B66E1D1B-CB7D-4B58-9430-5B21786DE2E6}" id="{27CC4477-F44C-47C1-9E73-E0CC9835FE6C}">
     <text>Has this changed?</text>
   </threadedComment>
-  <threadedComment ref="F87" dT="2024-12-20T15:47:50.11" personId="{B66E1D1B-CB7D-4B58-9430-5B21786DE2E6}" id="{EA9CD000-254B-42C0-8A79-94AD55225E73}" parentId="{27CC4477-F44C-47C1-9E73-E0CC9835FE6C}">
+  <threadedComment ref="F119" dT="2024-12-20T15:47:50.11" personId="{B66E1D1B-CB7D-4B58-9430-5B21786DE2E6}" id="{EA9CD000-254B-42C0-8A79-94AD55225E73}" parentId="{27CC4477-F44C-47C1-9E73-E0CC9835FE6C}">
     <text>Looks like a formula</text>
   </threadedComment>
 </ThreadedComments>
@@ -1235,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FCCD4D-CE26-40E6-81A9-7522D42312C3}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,42 +1435,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B1" t="s">
         <v>210</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>211</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" t="s">
         <v>212</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E1" t="s">
-        <v>213</v>
       </c>
       <c r="F1" t="s">
         <v>204</v>
       </c>
       <c r="G1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F2" t="s">
         <v>202</v>
@@ -1294,42 +1478,42 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1337,59 +1521,62 @@
         <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>225</v>
+        <v>241</v>
+      </c>
+      <c r="G7" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1397,16 +1584,16 @@
         <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
         <v>205</v>
@@ -1414,22 +1601,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>209</v>
+        <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,19 +1621,14 @@
         <v>168</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C10" t="s">
-        <v>155</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C10" s="1"/>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1457,116 +1636,89 @@
         <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" t="s">
-        <v>153</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>216</v>
+        <v>131</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>207</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="F12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="F13" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>221</v>
+        <v>143</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>223</v>
+        <v>137</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>239</v>
+        <v>133</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
       <c r="F16" t="s">
         <v>202</v>
@@ -1574,22 +1726,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>240</v>
+        <v>159</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1597,366 +1746,342 @@
         <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>217</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>224</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
-        <v>145</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>230</v>
+        <v>163</v>
       </c>
       <c r="E20" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>232</v>
+        <v>161</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>236</v>
+        <v>218</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>178</v>
       </c>
       <c r="C23" t="s">
-        <v>149</v>
+        <v>179</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B24" t="s">
-        <v>193</v>
+        <v>154</v>
       </c>
       <c r="C24" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="E24" t="s">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E25" t="s">
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27" t="s">
-        <v>141</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>235</v>
+        <v>132</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="E28" t="s">
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>87</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="F29" t="s">
-        <v>93</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>167</v>
       </c>
       <c r="E30" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>89</v>
+        <v>205</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>174</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="E32" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>176</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
       <c r="E34" t="s">
         <v>5</v>
       </c>
       <c r="F34" t="s">
-        <v>99</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
       <c r="E35" t="s">
         <v>5</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>137</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>101</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="C37" t="s">
-        <v>85</v>
+        <v>181</v>
       </c>
       <c r="E37" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F37" t="s">
         <v>202</v>
@@ -1964,16 +2089,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="E38" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
       <c r="F38" t="s">
         <v>202</v>
@@ -1981,135 +2103,126 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="E39" t="s">
         <v>5</v>
       </c>
       <c r="F39" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>182</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
       <c r="E41" t="s">
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>202</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>200</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="E42" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="E43" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="E44" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="E45" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>167</v>
       </c>
       <c r="E46" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="F46" t="s">
         <v>202</v>
@@ -2117,36 +2230,33 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B47" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
-        <v>5</v>
+        <v>134</v>
       </c>
       <c r="F47" t="s">
-        <v>26</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>135</v>
+        <v>201</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>198</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>199</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2154,50 +2264,59 @@
         <v>135</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>9</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="E50" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>200</v>
+        <v>42</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="E51" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F51" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -2205,16 +2324,19 @@
         <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C52" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="E52" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F52" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,10 +2344,13 @@
         <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
@@ -2239,10 +2364,13 @@
         <v>135</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>38</v>
+        <v>55</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="E54" t="s">
         <v>2</v>
@@ -2256,16 +2384,19 @@
         <v>135</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>53</v>
+        <v>7</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="E55" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F55" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2273,16 +2404,16 @@
         <v>135</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2290,16 +2421,16 @@
         <v>135</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,16 +2438,16 @@
         <v>135</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C58" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E58" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F58" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2324,16 +2455,16 @@
         <v>135</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="E59" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F59" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2341,16 +2472,16 @@
         <v>135</v>
       </c>
       <c r="B60" t="s">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="C60" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="E60" t="s">
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2358,16 +2489,16 @@
         <v>135</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
       <c r="E61" t="s">
         <v>5</v>
       </c>
       <c r="F61" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2375,16 +2506,16 @@
         <v>135</v>
       </c>
       <c r="B62" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="E62" t="s">
         <v>5</v>
       </c>
       <c r="F62" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2392,16 +2523,16 @@
         <v>135</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
       </c>
       <c r="F63" t="s">
-        <v>59</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2409,16 +2540,16 @@
         <v>135</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="C64" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="E64" t="s">
         <v>5</v>
       </c>
       <c r="F64" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -2426,16 +2557,16 @@
         <v>135</v>
       </c>
       <c r="B65" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="E65" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F65" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -2443,16 +2574,16 @@
         <v>135</v>
       </c>
       <c r="B66" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="E66" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2460,16 +2591,16 @@
         <v>135</v>
       </c>
       <c r="B67" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E67" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F67" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2477,16 +2608,16 @@
         <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E68" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F68" t="s">
-        <v>202</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2494,13 +2625,13 @@
         <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="E69" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F69" t="s">
         <v>202</v>
@@ -2511,13 +2642,13 @@
         <v>135</v>
       </c>
       <c r="B70" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="E70" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F70" t="s">
         <v>202</v>
@@ -2525,45 +2656,53 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B71" t="s">
-        <v>132</v>
-      </c>
-      <c r="C71" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>11</v>
+      </c>
       <c r="E71" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F71" t="s">
-        <v>202</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B72" t="s">
-        <v>132</v>
+        <v>14</v>
+      </c>
+      <c r="C72" t="s">
+        <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F72" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B73" t="s">
-        <v>132</v>
+        <v>17</v>
+      </c>
+      <c r="C73" t="s">
+        <v>18</v>
       </c>
       <c r="E73" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="F73" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2571,10 +2710,13 @@
         <v>135</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>12</v>
+      </c>
+      <c r="C74" t="s">
+        <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F74" t="s">
         <v>202</v>
@@ -2582,55 +2724,67 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>25</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
       </c>
       <c r="E75" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F75" t="s">
-        <v>202</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B76" t="s">
-        <v>132</v>
+        <v>21</v>
+      </c>
+      <c r="C76" t="s">
+        <v>22</v>
       </c>
       <c r="E76" t="s">
         <v>2</v>
       </c>
       <c r="F76" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="B77" t="s">
-        <v>132</v>
+        <v>23</v>
+      </c>
+      <c r="C77" t="s">
+        <v>24</v>
       </c>
       <c r="E77" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F77" t="s">
-        <v>202</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B78" t="s">
-        <v>131</v>
+        <v>35</v>
+      </c>
+      <c r="C78" t="s">
+        <v>36</v>
       </c>
       <c r="E78" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F78" t="s">
         <v>202</v>
@@ -2638,13 +2792,16 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>33</v>
+      </c>
+      <c r="C79" t="s">
+        <v>34</v>
       </c>
       <c r="E79" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F79" t="s">
         <v>202</v>
@@ -2652,13 +2809,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>37</v>
+      </c>
+      <c r="C80" t="s">
+        <v>38</v>
       </c>
       <c r="E80" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F80" t="s">
         <v>202</v>
@@ -2669,10 +2829,13 @@
         <v>135</v>
       </c>
       <c r="B81" t="s">
-        <v>131</v>
+        <v>52</v>
+      </c>
+      <c r="C81" t="s">
+        <v>53</v>
       </c>
       <c r="E81" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F81" t="s">
         <v>202</v>
@@ -2680,137 +2843,155 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
+        <v>50</v>
+      </c>
+      <c r="C82" t="s">
+        <v>51</v>
       </c>
       <c r="E82" t="s">
         <v>5</v>
       </c>
       <c r="F82" t="s">
-        <v>202</v>
+        <v>51</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B83" t="s">
-        <v>131</v>
+        <v>64</v>
+      </c>
+      <c r="C83" t="s">
+        <v>65</v>
       </c>
       <c r="E83" t="s">
         <v>5</v>
       </c>
       <c r="F83" t="s">
-        <v>202</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="B84" t="s">
-        <v>131</v>
+        <v>46</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
       </c>
       <c r="E84" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F84" t="s">
-        <v>202</v>
+        <v>47</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B85" t="s">
-        <v>183</v>
+        <v>60</v>
       </c>
       <c r="C85" t="s">
-        <v>184</v>
+        <v>61</v>
       </c>
       <c r="E85" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F85" t="s">
-        <v>205</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B86" t="s">
-        <v>185</v>
+        <v>48</v>
       </c>
       <c r="C86" t="s">
-        <v>186</v>
+        <v>49</v>
       </c>
       <c r="E86" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F86" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>187</v>
+        <v>62</v>
       </c>
       <c r="C87" t="s">
-        <v>188</v>
+        <v>63</v>
       </c>
       <c r="E87" t="s">
         <v>5</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>227</v>
+      <c r="F87" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
+        <v>44</v>
+      </c>
+      <c r="C88" t="s">
+        <v>45</v>
       </c>
       <c r="E88" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="F88" t="s">
-        <v>202</v>
+        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B89" t="s">
-        <v>129</v>
+        <v>58</v>
+      </c>
+      <c r="C89" t="s">
+        <v>59</v>
       </c>
       <c r="E89" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="F89" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B90" t="s">
-        <v>129</v>
+        <v>31</v>
+      </c>
+      <c r="C90" t="s">
+        <v>32</v>
       </c>
       <c r="E90" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>202</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2818,38 +2999,47 @@
         <v>135</v>
       </c>
       <c r="B91" t="s">
-        <v>129</v>
+        <v>27</v>
+      </c>
+      <c r="C91" t="s">
+        <v>28</v>
       </c>
       <c r="E91" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="F91" t="s">
-        <v>202</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B92" t="s">
-        <v>129</v>
+        <v>29</v>
+      </c>
+      <c r="C92" t="s">
+        <v>30</v>
       </c>
       <c r="E92" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="F92" t="s">
-        <v>202</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B93" t="s">
-        <v>129</v>
+        <v>110</v>
+      </c>
+      <c r="C93" t="s">
+        <v>111</v>
       </c>
       <c r="E93" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="F93" t="s">
         <v>202</v>
@@ -2857,13 +3047,16 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="B94" t="s">
-        <v>129</v>
+        <v>108</v>
+      </c>
+      <c r="C94" t="s">
+        <v>109</v>
       </c>
       <c r="E94" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
       <c r="F94" t="s">
         <v>202</v>
@@ -2874,13 +3067,13 @@
         <v>135</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C95" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E95" t="s">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="F95" t="s">
         <v>202</v>
@@ -2888,16 +3081,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
       <c r="C96" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
       <c r="E96" t="s">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="F96" t="s">
         <v>202</v>
@@ -2905,16 +3098,13 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B97" t="s">
-        <v>166</v>
-      </c>
-      <c r="C97" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="E97" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="F97" t="s">
         <v>202</v>
@@ -2922,16 +3112,13 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="B98" t="s">
-        <v>166</v>
-      </c>
-      <c r="C98" t="s">
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="E98" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="F98" t="s">
         <v>202</v>
@@ -2939,16 +3126,13 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>189</v>
+        <v>135</v>
       </c>
       <c r="B99" t="s">
-        <v>166</v>
-      </c>
-      <c r="C99" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="E99" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F99" t="s">
         <v>202</v>
@@ -2956,13 +3140,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B100" t="s">
-        <v>166</v>
+        <v>126</v>
       </c>
       <c r="C100" t="s">
-        <v>167</v>
+        <v>127</v>
       </c>
       <c r="E100" t="s">
         <v>128</v>
@@ -2973,16 +3157,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
-        <v>166</v>
-      </c>
-      <c r="C101" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="E101" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F101" t="s">
         <v>202</v>
@@ -2990,115 +3171,115 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B102" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="C102" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="E102" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="F102" t="s">
-        <v>205</v>
+        <v>67</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B103" t="s">
-        <v>142</v>
+        <v>70</v>
       </c>
       <c r="C103" t="s">
-        <v>173</v>
+        <v>71</v>
       </c>
       <c r="E103" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F103" t="s">
-        <v>205</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B104" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="C104" t="s">
-        <v>173</v>
+        <v>69</v>
       </c>
       <c r="E104" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F104" t="s">
-        <v>205</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="B105" t="s">
-        <v>142</v>
+        <v>72</v>
       </c>
       <c r="C105" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="E105" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F105" t="s">
-        <v>205</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B106" t="s">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="C106" t="s">
-        <v>175</v>
+        <v>77</v>
       </c>
       <c r="E106" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F106" t="s">
-        <v>175</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B107" t="s">
-        <v>176</v>
+        <v>74</v>
       </c>
       <c r="C107" t="s">
-        <v>177</v>
+        <v>75</v>
       </c>
       <c r="E107" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F107" t="s">
-        <v>177</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B108" t="s">
-        <v>169</v>
+        <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>170</v>
+        <v>4</v>
       </c>
       <c r="E108" t="s">
         <v>5</v>
@@ -3109,16 +3290,16 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B109" t="s">
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="C109" t="s">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F109" t="s">
         <v>205</v>
@@ -3126,197 +3307,203 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B110" t="s">
-        <v>171</v>
+        <v>120</v>
       </c>
       <c r="C110" t="s">
-        <v>172</v>
+        <v>121</v>
       </c>
       <c r="E110" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F110" t="s">
-        <v>219</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B111" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="C111" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="E111" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F111" t="s">
-        <v>219</v>
+        <v>123</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="B112" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C112" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="E112" t="s">
         <v>2</v>
       </c>
       <c r="F112" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="B113" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="C113" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="E113" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F113" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B114" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C114" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E114" t="s">
         <v>2</v>
       </c>
       <c r="F114" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B115" t="s">
-        <v>136</v>
-      </c>
-      <c r="C115" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E115" t="s">
         <v>2</v>
       </c>
       <c r="F115" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>189</v>
+      </c>
+      <c r="B116" t="s">
+        <v>131</v>
+      </c>
+      <c r="E116" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>189</v>
+      </c>
+      <c r="B117" t="s">
+        <v>183</v>
+      </c>
+      <c r="C117" t="s">
+        <v>184</v>
+      </c>
+      <c r="E117" t="s">
+        <v>16</v>
+      </c>
+      <c r="F117" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>182</v>
-      </c>
-      <c r="B116" t="s">
-        <v>180</v>
-      </c>
-      <c r="C116" t="s">
-        <v>181</v>
-      </c>
-      <c r="E116" t="s">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>189</v>
+      </c>
+      <c r="B118" t="s">
+        <v>185</v>
+      </c>
+      <c r="C118" t="s">
+        <v>186</v>
+      </c>
+      <c r="E118" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>189</v>
+      </c>
+      <c r="B119" t="s">
+        <v>187</v>
+      </c>
+      <c r="C119" t="s">
+        <v>188</v>
+      </c>
+      <c r="E119" t="s">
+        <v>5</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G119" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>189</v>
+      </c>
+      <c r="B120" t="s">
+        <v>129</v>
+      </c>
+      <c r="E120" t="s">
+        <v>130</v>
+      </c>
+      <c r="F120" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>189</v>
+      </c>
+      <c r="B121" t="s">
+        <v>166</v>
+      </c>
+      <c r="C121" t="s">
+        <v>167</v>
+      </c>
+      <c r="E121" t="s">
         <v>128</v>
       </c>
-      <c r="F116" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>190</v>
-      </c>
-      <c r="B117" t="s">
-        <v>180</v>
-      </c>
-      <c r="C117" t="s">
-        <v>181</v>
-      </c>
-      <c r="E117" t="s">
-        <v>128</v>
-      </c>
-      <c r="F117" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>168</v>
-      </c>
-      <c r="B118" t="s">
-        <v>133</v>
-      </c>
-      <c r="E118" t="s">
-        <v>134</v>
-      </c>
-      <c r="F118" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>182</v>
-      </c>
-      <c r="B119" t="s">
-        <v>133</v>
-      </c>
-      <c r="E119" t="s">
-        <v>134</v>
-      </c>
-      <c r="F119" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>201</v>
-      </c>
-      <c r="B120" t="s">
-        <v>133</v>
-      </c>
-      <c r="E120" t="s">
-        <v>134</v>
-      </c>
-      <c r="F120" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>135</v>
-      </c>
-      <c r="B121" t="s">
-        <v>133</v>
-      </c>
-      <c r="E121" t="s">
-        <v>134</v>
-      </c>
       <c r="F121" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>189</v>
       </c>
@@ -3330,165 +3517,177 @@
         <v>202</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>190</v>
       </c>
       <c r="B123" t="s">
-        <v>133</v>
+        <v>146</v>
+      </c>
+      <c r="C123" t="s">
+        <v>147</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="E123" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="F123" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B124" t="s">
-        <v>133</v>
+        <v>178</v>
+      </c>
+      <c r="C124" t="s">
+        <v>179</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="E124" t="s">
-        <v>134</v>
+        <v>16</v>
       </c>
       <c r="F124" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="B125" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C125" t="s">
-        <v>159</v>
+        <v>145</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="E125" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F125" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B126" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="C126" t="s">
-        <v>67</v>
+        <v>155</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="E126" t="s">
         <v>5</v>
       </c>
       <c r="F126" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B127" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="C127" t="s">
-        <v>71</v>
+        <v>153</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="E127" t="s">
         <v>5</v>
       </c>
       <c r="F127" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B128" t="s">
-        <v>68</v>
-      </c>
-      <c r="C128" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="E128" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F128" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B129" t="s">
-        <v>72</v>
-      </c>
-      <c r="C129" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="E129" t="s">
         <v>5</v>
       </c>
       <c r="F129" t="s">
-        <v>73</v>
+        <v>202</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B130" t="s">
-        <v>76</v>
-      </c>
-      <c r="C130" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="E130" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="F130" t="s">
-        <v>77</v>
+        <v>202</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>135</v>
+        <v>190</v>
       </c>
       <c r="B131" t="s">
-        <v>74</v>
+        <v>166</v>
       </c>
       <c r="C131" t="s">
-        <v>75</v>
+        <v>167</v>
       </c>
       <c r="E131" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="F131" t="s">
-        <v>75</v>
+        <v>202</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C132" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="E132" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F132" t="s">
         <v>205</v>
@@ -3496,13 +3695,13 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B133" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
       <c r="C133" t="s">
-        <v>139</v>
+        <v>170</v>
       </c>
       <c r="E133" t="s">
         <v>5</v>
@@ -3513,36 +3712,36 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B134" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="C134" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="E134" t="s">
         <v>5</v>
       </c>
       <c r="F134" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B135" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C135" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E135" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F135" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -3550,33 +3749,30 @@
         <v>190</v>
       </c>
       <c r="B136" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="C136" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="E136" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="F136" t="s">
-        <v>149</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B137" t="s">
-        <v>150</v>
-      </c>
-      <c r="C137" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="E137" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
       <c r="F137" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3584,33 +3780,33 @@
         <v>190</v>
       </c>
       <c r="B138" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C138" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E138" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F138" t="s">
-        <v>222</v>
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B139" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="C139" t="s">
-        <v>196</v>
+        <v>151</v>
       </c>
       <c r="E139" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F139" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -3618,16 +3814,19 @@
         <v>197</v>
       </c>
       <c r="B140" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C140" t="s">
-        <v>141</v>
+        <v>145</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="E140" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="F140" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -3635,98 +3834,92 @@
         <v>197</v>
       </c>
       <c r="B141" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C141" t="s">
-        <v>192</v>
+        <v>194</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="E141" t="s">
         <v>5</v>
       </c>
       <c r="F141" t="s">
-        <v>192</v>
+        <v>231</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B142" t="s">
-        <v>3</v>
-      </c>
-      <c r="C142" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="E142" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F142" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B143" t="s">
-        <v>198</v>
-      </c>
-      <c r="C143" t="s">
-        <v>199</v>
+        <v>131</v>
       </c>
       <c r="E143" t="s">
         <v>5</v>
       </c>
       <c r="F143" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="B144" t="s">
-        <v>164</v>
-      </c>
-      <c r="C144" t="s">
-        <v>165</v>
+        <v>129</v>
       </c>
       <c r="E144" t="s">
-        <v>2</v>
+        <v>130</v>
       </c>
       <c r="F144" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="B145" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C145" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E145" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="F145" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="E146" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="F146" t="s">
         <v>205</v>
@@ -3734,13 +3927,13 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B147" t="s">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="C147" t="s">
-        <v>1</v>
+        <v>137</v>
       </c>
       <c r="E147" t="s">
         <v>2</v>
@@ -3751,90 +3944,107 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B148" t="s">
-        <v>120</v>
-      </c>
-      <c r="C148" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="E148" t="s">
-        <v>2</v>
+        <v>134</v>
       </c>
       <c r="F148" t="s">
-        <v>121</v>
+        <v>202</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B149" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="C149" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="E149" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F149" t="s">
-        <v>123</v>
+        <v>205</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B150" t="s">
-        <v>118</v>
+        <v>195</v>
       </c>
       <c r="C150" t="s">
-        <v>119</v>
+        <v>196</v>
       </c>
       <c r="E150" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F150" t="s">
-        <v>119</v>
+        <v>229</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B151" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="C151" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="E151" t="s">
         <v>5</v>
       </c>
       <c r="F151" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
       <c r="B152" t="s">
-        <v>124</v>
+        <v>191</v>
       </c>
       <c r="C152" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
       <c r="E152" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F152" t="s">
-        <v>125</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D152 F2:F152">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND(NOT(ISBLANK($D2)), $F2 &lt;&gt;"NOT USED", $F2 &lt;&gt; "PARAMETER", $D2 &lt;&gt; $F2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F152">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND($F2 &lt;&gt; "NOT USED", $F2 &lt;&gt; "PARAMETER", OR(ISBLANK($D2), $F2 = $D2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D152">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(NOT(ISBLANK($D2)), OR($F2 = "NOT USED", $F2 = "PARAMETER"))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C152">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>AND(NOT(ISBLANK($C2)), ISBLANK($D2), OR($F2 = "NOT USED", $F2 = "PARAMETER"))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Interim commit before merge
</commit_message>
<xml_diff>
--- a/data/Survey123_Field Names and Aliases_20241220.xlsx
+++ b/data/Survey123_Field Names and Aliases_20241220.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\manniongeo\projects\nwfwmd\2015-01-13_gis_support\github\Hydrologic-Monitoring-Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B11D9DE-91E4-4283-958F-FD4A89A816AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F058178F-6179-4ADC-A348-EF37ACCC2FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17730" xr2:uid="{2EC705E7-C833-41D9-B7F8-0755F5ED5DAB}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="252">
   <si>
     <t>VisitDate</t>
   </si>
@@ -784,32 +784,42 @@
     <t>Keep existing geodatabase aliases</t>
   </si>
   <si>
+    <t>Verify "Date" vs "Timestamp"</t>
+  </si>
+  <si>
+    <t>Omit "Issue" prefix</t>
+  </si>
+  <si>
+    <t>Omit "Conductivity" prefix</t>
+  </si>
+  <si>
+    <t>Omit "Stage" prefix</t>
+  </si>
+  <si>
+    <t>Omit "Temperature" prefix</t>
+  </si>
+  <si>
     <t>Specific Conductance Sensor Failed
-Verify; seems to flip yes/no values</t>
-  </si>
-  <si>
-    <t>Verify; seems to flip yes/no values</t>
-  </si>
-  <si>
-    <t>Should we change "Rainfall" to "Tipping"?</t>
-  </si>
-  <si>
-    <t>Verify "Date" vs "Timestamp"</t>
-  </si>
-  <si>
-    <t>Omit "Issue" prefix</t>
-  </si>
-  <si>
-    <t>Omit "Conductivity" prefix</t>
-  </si>
-  <si>
-    <t>Omit "Stage" prefix</t>
-  </si>
-  <si>
-    <t>Omit "Temperature" prefix</t>
-  </si>
-  <si>
-    <t>Verify that we should omit "(feet")</t>
+Verify; seems to flip yes/no values: KEEP
+OMIT PREFIX "SPECIFIC CONDUCTANCE"</t>
+  </si>
+  <si>
+    <t>CHANGE SURVEY123 ALIAS TO MATCH AQUARIUS</t>
+  </si>
+  <si>
+    <t>Verify "Date" vs "Timestamp"
+KEEP DATE</t>
+  </si>
+  <si>
+    <t>Should we change "Rainfall" to "Tipping"?
+YES</t>
+  </si>
+  <si>
+    <t>Verify; seems to flip yes/no values
+CHANGE COLUMN NAME TO "CHANGES TO EQUIPMENT"
+ALSO LOOK AT DEFAULT VALUE; SHOULD BE "NO"
+UPDATE WORKFLOW DIAGRAM TO REVERSE ARROWS / UPDATE DATA SOURCE
+NEEDS NEW TICKET; INCLUDE SARAH FOR SURVEY123 CONFIG CHANGE</t>
   </si>
 </sst>
 </file>
@@ -845,7 +855,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -855,6 +865,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -879,6 +895,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1309,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85FCCD4D-CE26-40E6-81A9-7522D42312C3}">
   <dimension ref="A1:G152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F150" sqref="F150"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1526,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>168</v>
       </c>
@@ -1526,7 +1546,7 @@
         <v>240</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1569,7 +1589,7 @@
         <v>213</v>
       </c>
       <c r="G14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1592,7 +1612,7 @@
         <v>205</v>
       </c>
       <c r="G15" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1615,10 +1635,10 @@
         <v>214</v>
       </c>
       <c r="G16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -1638,7 +1658,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>168</v>
       </c>
@@ -1658,7 +1678,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -1675,7 +1695,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>168</v>
       </c>
@@ -1692,7 +1712,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>168</v>
       </c>
@@ -1709,7 +1729,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -1723,7 +1743,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>182</v>
       </c>
@@ -1737,7 +1757,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -1751,7 +1771,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -1768,7 +1788,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>182</v>
       </c>
@@ -1785,7 +1805,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>182</v>
       </c>
@@ -1802,7 +1822,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>182</v>
       </c>
@@ -1819,7 +1839,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>182</v>
       </c>
@@ -1836,7 +1856,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>182</v>
       </c>
@@ -1852,8 +1872,11 @@
       <c r="F30" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>182</v>
       </c>
@@ -1870,7 +1893,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>182</v>
       </c>
@@ -1975,7 +1998,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>182</v>
       </c>
@@ -1991,8 +2014,8 @@
       <c r="F38" t="s">
         <v>220</v>
       </c>
-      <c r="G38" t="s">
-        <v>245</v>
+      <c r="G38" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2072,7 +2095,7 @@
         <v>224</v>
       </c>
       <c r="G42" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3004,7 +3027,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>135</v>
       </c>
@@ -3023,8 +3046,8 @@
       <c r="F98" t="s">
         <v>208</v>
       </c>
-      <c r="G98" t="s">
-        <v>243</v>
+      <c r="G98" s="5" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -3126,7 +3149,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>135</v>
       </c>
@@ -3142,8 +3165,8 @@
       <c r="F105" t="s">
         <v>77</v>
       </c>
-      <c r="G105" t="s">
-        <v>244</v>
+      <c r="G105" s="4" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -3644,10 +3667,10 @@
         <v>226</v>
       </c>
       <c r="G135" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>190</v>
       </c>
@@ -3663,8 +3686,8 @@
       <c r="F136" t="s">
         <v>220</v>
       </c>
-      <c r="G136" t="s">
-        <v>245</v>
+      <c r="G136" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -3687,7 +3710,7 @@
         <v>227</v>
       </c>
       <c r="G137" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -3805,9 +3828,6 @@
       <c r="F144" t="s">
         <v>205</v>
       </c>
-      <c r="G144" t="s">
-        <v>250</v>
-      </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
@@ -3874,7 +3894,7 @@
         <v>229</v>
       </c>
       <c r="G148" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>